<commit_message>
se planteo un controlador LQI
Presenta posible buena respuesta
</commit_message>
<xml_diff>
--- a/relacion_Voltaje_vs_corriente.xlsx
+++ b/relacion_Voltaje_vs_corriente.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan\Documents\GitHub\Proyecto_de_Graduacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C08907-26D1-47D1-B958-FCB58AB74765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF88A398-8DAE-4F1C-A342-2B31CBE85577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3637F35-3F90-4F35-8F95-653C89851009}"/>
   </bookViews>
@@ -45,10 +45,10 @@
     <t>practico</t>
   </si>
   <si>
-    <t>Voltaje/corriente</t>
+    <t>corriente aproximada con regrecion</t>
   </si>
   <si>
-    <t>corriente aproximada con regrecion</t>
+    <t>corriente/voltaje</t>
   </si>
 </sst>
 </file>
@@ -56,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -89,10 +89,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -246,32 +246,35 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.18</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.21</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.32500000000000001</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.375</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
@@ -279,32 +282,35 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$11</c:f>
+              <c:f>Sheet1!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.38750000000000001</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.4375</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.51249999999999996</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.5625</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.63749999999999996</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.66874999999999996</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -343,34 +349,115 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.5269095729845991E-3"/>
+                  <c:y val="0.22020227865487452"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-GT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.18</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.21</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.32500000000000001</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.375</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
@@ -378,32 +465,35 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$11</c:f>
+              <c:f>Sheet1!$C$3:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.252</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.29399999999999998</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.42</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.45499999999999996</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.48999999999999994</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.52499999999999991</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.55999999999999994</c:v>
                 </c:pt>
               </c:numCache>
@@ -1531,17 +1621,17 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D23"/>
+      <selection activeCell="A16" sqref="A16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1662,84 +1752,84 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <f>(B4-0.1455)/1.3984</f>
-        <v>0.17305491990846683</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="A16" s="1">
+        <f>(B4-0.046)/1.7124</f>
+        <v>0.19942770380752164</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <f t="shared" ref="A17:A29" si="1">(B5-0.1455)/1.3984</f>
-        <v>0.20881006864988561</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="1">
+        <f t="shared" ref="A17:A23" si="1">(B5-0.046)/1.7124</f>
+        <v>0.22862648913805186</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <f t="shared" si="1"/>
-        <v>0.26244279176201368</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+        <v>0.27242466713384722</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <f t="shared" si="1"/>
-        <v>0.29819794050343251</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+        <v>0.3016234524643775</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <f t="shared" si="1"/>
-        <v>0.32501430205949655</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+        <v>0.32352254146227516</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <f t="shared" si="1"/>
-        <v>0.35183066361556059</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+        <v>0.34542163046017282</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <f t="shared" si="1"/>
-        <v>0.37417763157894735</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+        <v>0.36367087129175424</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <f t="shared" si="1"/>
-        <v>0.39652459954233404</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+        <v>0.38192011212333565</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>